<commit_message>
Whole Lot Of Changes
</commit_message>
<xml_diff>
--- a/findbyfilewebelement/src/test/resources/excel/ValidMultiplePageData.xlsx
+++ b/findbyfilewebelement/src/test/resources/excel/ValidMultiplePageData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="3870" windowWidth="14670" windowHeight="6750" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2190" windowWidth="14490" windowHeight="6750" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -60,13 +61,13 @@
     <t>fourthField</t>
   </si>
   <si>
-    <t>file.pagefactory.excel.ExcelFileMultiplePageTest$FirstMultiplePage</t>
-  </si>
-  <si>
-    <t>file.pagefactory.excel.ExcelFileMultiplePageTest$ThirdMultiplePage</t>
-  </si>
-  <si>
-    <t>file.pagefactory.excel.ExcelFileMultiplePageTest$SecondMultiplePage</t>
+    <t>file.pagefactory.excel.ExcelFileProcessorMultiplePageTest$FirstMultiplePage</t>
+  </si>
+  <si>
+    <t>file.pagefactory.excel.ExcelFileProcessorMultiplePageTest$ThirdMultiplePage</t>
+  </si>
+  <si>
+    <t>file.pagefactory.excel.ExcelFileProcessorMultiplePageTest$SecondMultiplePage</t>
   </si>
 </sst>
 </file>
@@ -425,7 +426,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>